<commit_message>
verwerk gegevens van de voorbeelden A t/m G in het kennismodel
</commit_message>
<xml_diff>
--- a/NVWA DTV/Voorbeelden uitgewerkt.xlsx
+++ b/NVWA DTV/Voorbeelden uitgewerkt.xlsx
@@ -4,21 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="20610" windowHeight="11640" activeTab="4"/>
+    <workbookView xWindow="120" yWindow="36" windowWidth="20616" windowHeight="11640" tabRatio="760" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
-    <sheet name="Tijdregistraties" sheetId="2" r:id="rId2"/>
-    <sheet name="TijdvakResultaten" sheetId="4" r:id="rId3"/>
-    <sheet name="Dagverantwoordingen" sheetId="3" r:id="rId4"/>
-    <sheet name="Resultaat" sheetId="5" r:id="rId5"/>
+    <sheet name="pop tijdregistraties" sheetId="2" r:id="rId2"/>
+    <sheet name="pop tijdvakresultaten" sheetId="4" r:id="rId3"/>
+    <sheet name="pop dagverantwoordingen" sheetId="3" r:id="rId4"/>
+    <sheet name="pop resultaten" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="244">
   <si>
     <t>Voorbeelden</t>
   </si>
@@ -260,9 +260,6 @@
     <t>Tijdsduur</t>
   </si>
   <si>
-    <t>Periode</t>
-  </si>
-  <si>
     <t>Uren</t>
   </si>
   <si>
@@ -299,15 +296,6 @@
     <t>Persoon</t>
   </si>
   <si>
-    <t>dagverantwoordingVanBetaalperiode</t>
-  </si>
-  <si>
-    <t>Betaalperiode</t>
-  </si>
-  <si>
-    <t>periodeverantwoordingPeriode</t>
-  </si>
-  <si>
     <t>periodeverantwoording</t>
   </si>
   <si>
@@ -320,18 +308,12 @@
     <t>DV6</t>
   </si>
   <si>
-    <t>p201411</t>
-  </si>
-  <si>
     <t>p2</t>
   </si>
   <si>
     <t>DV10</t>
   </si>
   <si>
-    <t>p201409</t>
-  </si>
-  <si>
     <t>pv13</t>
   </si>
   <si>
@@ -759,6 +741,15 @@
   </si>
   <si>
     <t>res11</t>
+  </si>
+  <si>
+    <t>dagverantwoording</t>
+  </si>
+  <si>
+    <t>leeg</t>
+  </si>
+  <si>
+    <t>Leeg</t>
   </si>
 </sst>
 </file>
@@ -1186,18 +1177,18 @@
       <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="25.140625" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="25.109375" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" customWidth="1"/>
+    <col min="7" max="7" width="19.109375" style="8" customWidth="1"/>
     <col min="8" max="8" width="27" style="8" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" customWidth="1"/>
+    <col min="9" max="9" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:61">
       <c r="A1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:61">
@@ -1207,7 +1198,7 @@
     </row>
     <row r="4" spans="1:61">
       <c r="A4" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>32</v>
@@ -1217,7 +1208,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:61" ht="30">
+    <row r="5" spans="1:61" ht="28.8">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -1305,7 +1296,7 @@
     </row>
     <row r="7" spans="1:61" s="4" customFormat="1">
       <c r="A7" s="4" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B7" s="2">
         <v>0.33333333333333331</v>
@@ -1324,7 +1315,7 @@
     </row>
     <row r="8" spans="1:61" s="4" customFormat="1">
       <c r="A8" s="4" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B8" s="2">
         <v>0.51041666666666663</v>
@@ -1343,7 +1334,7 @@
     </row>
     <row r="9" spans="1:61" s="4" customFormat="1">
       <c r="A9" s="4" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B9" s="2">
         <v>0.54166666666666663</v>
@@ -1394,7 +1385,7 @@
     </row>
     <row r="14" spans="1:61" s="4" customFormat="1">
       <c r="A14" s="4" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>33</v>
@@ -1438,7 +1429,7 @@
     </row>
     <row r="17" spans="1:9" s="4" customFormat="1">
       <c r="A17" s="4" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B17" s="2">
         <v>0.33333333333333331</v>
@@ -1457,7 +1448,7 @@
     </row>
     <row r="18" spans="1:9" s="4" customFormat="1">
       <c r="A18" s="4" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B18" s="2">
         <v>0.51041666666666663</v>
@@ -1474,9 +1465,9 @@
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
     </row>
-    <row r="19" spans="1:9" s="4" customFormat="1" ht="30">
+    <row r="19" spans="1:9" s="4" customFormat="1" ht="28.8">
       <c r="A19" s="4" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B19" s="2">
         <v>0.54166666666666663</v>
@@ -1517,7 +1508,7 @@
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
     </row>
-    <row r="22" spans="1:9" s="4" customFormat="1" ht="30">
+    <row r="22" spans="1:9" s="4" customFormat="1" ht="28.8">
       <c r="B22" s="5"/>
       <c r="C22" s="5" t="s">
         <v>15</v>
@@ -1545,7 +1536,7 @@
     </row>
     <row r="25" spans="1:9" s="4" customFormat="1">
       <c r="A25" s="4" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>34</v>
@@ -1589,7 +1580,7 @@
     </row>
     <row r="28" spans="1:9" s="4" customFormat="1">
       <c r="A28" s="4" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B28" s="2">
         <v>0.33333333333333331</v>
@@ -1608,7 +1599,7 @@
     </row>
     <row r="29" spans="1:9" s="4" customFormat="1">
       <c r="A29" s="4" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B29" s="2">
         <v>0.5</v>
@@ -1627,7 +1618,7 @@
     </row>
     <row r="30" spans="1:9" s="4" customFormat="1">
       <c r="A30" s="4" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B30" s="2">
         <v>0.54166666666666663</v>
@@ -1646,7 +1637,7 @@
     </row>
     <row r="31" spans="1:9" s="4" customFormat="1">
       <c r="A31" s="4" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B31" s="2">
         <v>0.58333333333333337</v>
@@ -1829,7 +1820,7 @@
       <c r="G43" s="9"/>
       <c r="H43" s="9"/>
     </row>
-    <row r="44" spans="2:10" s="4" customFormat="1" ht="30">
+    <row r="44" spans="2:10" s="4" customFormat="1">
       <c r="B44" s="2">
         <v>0.52083333333333337</v>
       </c>
@@ -1847,7 +1838,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="45" spans="2:10" s="4" customFormat="1" ht="60">
+    <row r="45" spans="2:10" s="4" customFormat="1" ht="43.2">
       <c r="B45" s="2">
         <v>0.5625</v>
       </c>
@@ -2213,7 +2204,7 @@
       </c>
       <c r="H72" s="9"/>
     </row>
-    <row r="73" spans="2:10" s="4" customFormat="1" ht="30">
+    <row r="73" spans="2:10" s="4" customFormat="1" ht="28.8">
       <c r="B73" s="2">
         <v>0.70833333333333337</v>
       </c>
@@ -2236,7 +2227,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="74" spans="2:10" s="4" customFormat="1" ht="30">
+    <row r="74" spans="2:10" s="4" customFormat="1">
       <c r="B74" s="2">
         <v>0.91666666666666663</v>
       </c>
@@ -2382,14 +2373,14 @@
       <c r="G88" s="9"/>
       <c r="H88" s="9"/>
     </row>
-    <row r="89" spans="2:8" s="4" customFormat="1" ht="15.75">
+    <row r="89" spans="2:8" s="4" customFormat="1" ht="15.6">
       <c r="B89" s="7" t="s">
         <v>44</v>
       </c>
       <c r="G89" s="9"/>
       <c r="H89" s="9"/>
     </row>
-    <row r="90" spans="2:8" s="4" customFormat="1" ht="15.75">
+    <row r="90" spans="2:8" s="4" customFormat="1" ht="15.6">
       <c r="B90" s="6" t="s">
         <v>39</v>
       </c>
@@ -2401,28 +2392,28 @@
       <c r="G91" s="9"/>
       <c r="H91" s="9"/>
     </row>
-    <row r="92" spans="2:8" s="4" customFormat="1" ht="15.75">
+    <row r="92" spans="2:8" s="4" customFormat="1" ht="15.6">
       <c r="B92" s="6" t="s">
         <v>40</v>
       </c>
       <c r="G92" s="9"/>
       <c r="H92" s="9"/>
     </row>
-    <row r="93" spans="2:8" s="4" customFormat="1" ht="15.75">
+    <row r="93" spans="2:8" s="4" customFormat="1" ht="15.6">
       <c r="B93" s="6" t="s">
         <v>41</v>
       </c>
       <c r="G93" s="9"/>
       <c r="H93" s="9"/>
     </row>
-    <row r="94" spans="2:8" s="4" customFormat="1" ht="15.75">
+    <row r="94" spans="2:8" s="4" customFormat="1" ht="15.6">
       <c r="B94" s="6" t="s">
         <v>42</v>
       </c>
       <c r="G94" s="9"/>
       <c r="H94" s="9"/>
     </row>
-    <row r="95" spans="2:8" s="4" customFormat="1" ht="15.75">
+    <row r="95" spans="2:8" s="4" customFormat="1" ht="15.6">
       <c r="B95" s="6" t="s">
         <v>43</v>
       </c>
@@ -3686,702 +3677,759 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" customWidth="1"/>
+    <col min="6" max="6" width="14.5546875" customWidth="1"/>
+    <col min="7" max="7" width="14.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" t="s">
-        <v>65</v>
+    <row r="1" spans="1:9">
+      <c r="B1" t="s">
+        <v>85</v>
       </c>
       <c r="C1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" t="s">
         <v>86</v>
       </c>
-      <c r="D1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F1" t="s">
-        <v>76</v>
-      </c>
-      <c r="G1" t="s">
-        <v>77</v>
-      </c>
-      <c r="H1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B2" t="s">
-        <v>88</v>
-      </c>
       <c r="C2" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="D2" t="s">
         <v>78</v>
       </c>
       <c r="E2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F2" t="s">
-        <v>79</v>
+        <v>5</v>
       </c>
       <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>139</v>
+      </c>
       <c r="B3" t="s">
-        <v>145</v>
-      </c>
-      <c r="C3" t="s">
-        <v>135</v>
+        <v>129</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.33333333333333331</v>
       </c>
       <c r="D3" s="2">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.17708333333333334</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E4" s="2">
+        <v>3.125E-2</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C6" s="2">
         <v>0.33333333333333331</v>
       </c>
-      <c r="E3" s="2">
+      <c r="D6" s="2">
         <v>0.51041666666666663</v>
       </c>
-      <c r="F3" s="2">
+      <c r="E6" s="2">
         <v>0.17708333333333334</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="G6" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>143</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E7" s="2">
+        <v>3.125E-2</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>144</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>157</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>158</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E10" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>159</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E11" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>160</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.125</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="4" customFormat="1">
+      <c r="A13" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="E13" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="4" customFormat="1">
+      <c r="A14" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E14" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="4" customFormat="1">
+      <c r="A15" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="B4" t="s">
-        <v>146</v>
-      </c>
-      <c r="C4" t="s">
-        <v>135</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0.51041666666666663</v>
-      </c>
-      <c r="E4" s="2">
+      <c r="B15" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="E15" s="2">
+        <v>3.125E-2</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="4" customFormat="1">
+      <c r="A16" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.13541666666666666</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="4" customFormat="1">
+      <c r="A17" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="E17" s="2">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="4" customFormat="1">
+      <c r="A18" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.5625</v>
+      </c>
+      <c r="E18" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="4" customFormat="1">
+      <c r="A19" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.5625</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E19" s="2">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="4" customFormat="1">
+      <c r="A20" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="E20" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="4" customFormat="1">
+      <c r="A21" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E21" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="4" customFormat="1">
+      <c r="A22" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="E22" s="2">
+        <v>3.125E-2</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="4" customFormat="1">
+      <c r="A23" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0.13541666666666666</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" s="4" customFormat="1">
+      <c r="A24" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="E24" s="2">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" s="4" customFormat="1">
+      <c r="A25" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.5625</v>
+      </c>
+      <c r="E25" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" s="4" customFormat="1">
+      <c r="A26" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0.5625</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E26" s="2">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" s="4" customFormat="1">
+      <c r="A27" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="4" customFormat="1">
+      <c r="A28" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D28" s="2">
         <v>0.54166666666666663</v>
       </c>
-      <c r="F4" s="2">
-        <v>3.125E-2</v>
-      </c>
-      <c r="G4" s="4" t="s">
+      <c r="E28" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F28" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="B5" t="s">
-        <v>147</v>
-      </c>
-      <c r="C5" t="s">
-        <v>135</v>
-      </c>
-      <c r="D5" s="2">
+      <c r="G28" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" s="4" customFormat="1">
+      <c r="A29" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="C29" s="2">
         <v>0.54166666666666663</v>
       </c>
-      <c r="E5" s="2">
-        <v>0.79166666666666663</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="G5" s="4" t="s">
+      <c r="D29" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E29" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F29" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="B6" t="s">
-        <v>148</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0.51041666666666663</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0.17708333333333334</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="B7" t="s">
-        <v>149</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0.51041666666666663</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="F7" s="2">
-        <v>3.125E-2</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="B8" t="s">
-        <v>150</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="E8" s="2">
-        <v>0.79166666666666663</v>
-      </c>
-      <c r="F8" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="B9" t="s">
-        <v>163</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="E9" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="F9" s="2">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="B10" t="s">
-        <v>164</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="D10" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="E10" s="2">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="F10" s="2">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="B11" t="s">
-        <v>165</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="D11" s="2">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="E11" s="2">
+      <c r="G29" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" s="4" customFormat="1">
+      <c r="A30" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="C30" s="2">
         <v>0.58333333333333337</v>
       </c>
-      <c r="F11" s="2">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="B12" t="s">
-        <v>166</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="D12" s="2">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="E12" s="2">
+      <c r="D30" s="2">
         <v>0.70833333333333337</v>
       </c>
-      <c r="F12" s="2">
+      <c r="E30" s="2">
         <v>0.125</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="F30" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H12" s="4" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" s="4" customFormat="1">
-      <c r="B13" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="D13" s="2">
-        <v>0.20833333333333334</v>
-      </c>
-      <c r="E13" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="F13" s="2">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" s="4" customFormat="1">
-      <c r="B14" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="D14" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="E14" s="2">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="F14" s="2">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" s="4" customFormat="1">
-      <c r="B15" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="D15" s="2">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0.36458333333333331</v>
-      </c>
-      <c r="F15" s="2">
-        <v>3.125E-2</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" s="4" customFormat="1">
-      <c r="B16" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="D16" s="2">
-        <v>0.36458333333333331</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="F16" s="2">
-        <v>0.13541666666666666</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" s="4" customFormat="1">
-      <c r="B17" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="D17" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="E17" s="2">
-        <v>0.52083333333333337</v>
-      </c>
-      <c r="F17" s="2">
+      <c r="G30" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" s="4" customFormat="1">
+      <c r="A31" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.8125</v>
+      </c>
+      <c r="E31" s="2">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" s="4" customFormat="1">
+      <c r="A32" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="C32" s="2">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0.9375</v>
+      </c>
+      <c r="E32" s="2">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="G17" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" s="4" customFormat="1">
-      <c r="B18" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="D18" s="2">
-        <v>0.52083333333333337</v>
-      </c>
-      <c r="E18" s="2">
-        <v>0.5625</v>
-      </c>
-      <c r="F18" s="2">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" s="4" customFormat="1">
-      <c r="B19" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="D19" s="2">
-        <v>0.5625</v>
-      </c>
-      <c r="E19" s="2">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="F19" s="2">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" s="4" customFormat="1">
-      <c r="B20" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D20" s="2">
-        <v>0.20833333333333334</v>
-      </c>
-      <c r="E20" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="F20" s="2">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" s="4" customFormat="1">
-      <c r="B21" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D21" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="E21" s="2">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="F21" s="2">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" s="4" customFormat="1">
-      <c r="B22" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D22" s="2">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="E22" s="2">
-        <v>0.36458333333333331</v>
-      </c>
-      <c r="F22" s="2">
-        <v>3.125E-2</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" s="4" customFormat="1">
-      <c r="B23" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D23" s="2">
-        <v>0.36458333333333331</v>
-      </c>
-      <c r="E23" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="F23" s="2">
-        <v>0.13541666666666666</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" s="4" customFormat="1">
-      <c r="B24" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D24" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="E24" s="2">
-        <v>0.52083333333333337</v>
-      </c>
-      <c r="F24" s="2">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" s="4" customFormat="1">
-      <c r="B25" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D25" s="2">
-        <v>0.52083333333333337</v>
-      </c>
-      <c r="E25" s="2">
-        <v>0.5625</v>
-      </c>
-      <c r="F25" s="2">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" s="4" customFormat="1">
-      <c r="B26" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D26" s="2">
-        <v>0.5625</v>
-      </c>
-      <c r="E26" s="2">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="F26" s="2">
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" s="4" customFormat="1">
-      <c r="B27" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="D27" s="2">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="E27" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="F27" s="2">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" s="4" customFormat="1">
-      <c r="B28" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="D28" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="E28" s="2">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="F28" s="2">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" s="4" customFormat="1">
-      <c r="B29" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="D29" s="2">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="E29" s="2">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="F29" s="2">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" s="4" customFormat="1">
-      <c r="B30" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="D30" s="2">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="E30" s="2">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="F30" s="2">
-        <v>0.125</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" s="4" customFormat="1">
-      <c r="B31" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="D31" s="2">
-        <v>0.70833333333333337</v>
-      </c>
-      <c r="E31" s="2">
-        <v>0.8125</v>
-      </c>
-      <c r="F31" s="2">
-        <v>0.10416666666666667</v>
-      </c>
-      <c r="G31" s="4" t="s">
+      <c r="F32" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="32" spans="2:7" s="4" customFormat="1">
-      <c r="B32" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="D32" s="2">
-        <v>0.91666666666666663</v>
-      </c>
-      <c r="E32" s="2">
-        <v>0.9375</v>
-      </c>
-      <c r="F32" s="2">
-        <v>2.0833333333333332E-2</v>
-      </c>
       <c r="G32" s="4" t="s">
-        <v>26</v>
+        <v>180</v>
       </c>
     </row>
     <row r="33" s="4" customFormat="1"/>
@@ -4395,93 +4443,96 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="9.42578125" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="4"/>
+    <col min="2" max="2" width="9.44140625" customWidth="1"/>
+    <col min="4" max="4" width="22.109375" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="B1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="H1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" t="s">
         <v>138</v>
       </c>
-      <c r="C1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D1" t="s">
-        <v>141</v>
-      </c>
-      <c r="E1" t="s">
-        <v>142</v>
-      </c>
-      <c r="F1" t="s">
-        <v>143</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B3" t="s">
         <v>139</v>
       </c>
-      <c r="D2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E2" t="s">
-        <v>83</v>
-      </c>
-      <c r="F2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
-        <v>151</v>
-      </c>
-      <c r="B3" t="s">
-        <v>145</v>
-      </c>
       <c r="C3" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F3" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="G3" s="2">
         <v>0.17708333333333334</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B4" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C4" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>11</v>
@@ -4490,90 +4541,90 @@
         <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="G4" s="2">
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B5" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C5" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F5" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="G5" s="2">
         <v>0.20833333333333334</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B6" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C6" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F6" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="G6" s="2">
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="B7" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C7" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F7" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="G7" s="2">
         <v>0.17708333333333334</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B8" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C8" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>11</v>
@@ -4582,113 +4633,113 @@
         <v>7</v>
       </c>
       <c r="F8" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="G8" s="2">
         <v>3.125E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B9" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C9" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F9" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="G9" s="2">
         <v>0.15625</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B10" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C10" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E10" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="F10" t="s">
         <v>170</v>
-      </c>
-      <c r="F10" t="s">
-        <v>176</v>
       </c>
       <c r="G10" s="2">
         <v>5.2083333333333336E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B11" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C11" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E11" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="F11" t="s">
         <v>170</v>
-      </c>
-      <c r="F11" t="s">
-        <v>176</v>
       </c>
       <c r="G11" s="2">
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B12" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C12" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F12" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="G12" s="2">
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B13" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="C13" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>11</v>
@@ -4697,76 +4748,76 @@
         <v>7</v>
       </c>
       <c r="F13" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="G13" s="2">
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B14" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="C14" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F14" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="G14" s="2">
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B15" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C15" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="F15" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="G15" s="2">
         <v>0.125</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="C16" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="G16" s="2">
         <v>4.1666666666666664E-2</v>
@@ -4774,22 +4825,22 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="C17" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="G17" s="2">
         <v>8.3333333333333329E-2</v>
@@ -4797,22 +4848,22 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="C18" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="G18" s="2">
         <v>3.125E-2</v>
@@ -4820,22 +4871,22 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="C19" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="G19" s="2">
         <v>0.13541666666666666</v>
@@ -4843,13 +4894,13 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="C20" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>20</v>
@@ -4858,7 +4909,7 @@
         <v>7</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="G20" s="2">
         <v>2.0833333333333332E-2</v>
@@ -4866,22 +4917,22 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="C21" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="G21" s="2">
         <v>4.1666666666666664E-2</v>
@@ -4889,22 +4940,22 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="C22" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="G22" s="2">
         <v>2.0833333333333332E-2</v>
@@ -4912,22 +4963,22 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="C23" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="G23" s="2">
         <v>4.1666666666666664E-2</v>
@@ -4935,22 +4986,22 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C24" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="G24" s="2">
         <v>8.3333333333333329E-2</v>
@@ -4958,22 +5009,22 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="C25" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="G25" s="2">
         <v>3.125E-2</v>
@@ -4981,22 +5032,22 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C26" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="G26" s="2">
         <v>0.13541666666666666</v>
@@ -5004,13 +5055,13 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="C27" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>20</v>
@@ -5019,7 +5070,7 @@
         <v>7</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="G27" s="2">
         <v>2.0833333333333332E-2</v>
@@ -5027,22 +5078,22 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="C28" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="G28" s="2">
         <v>4.1666666666666664E-2</v>
@@ -5050,22 +5101,22 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="C29" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="G29" s="2">
         <v>2.0833333333333332E-2</v>
@@ -5073,22 +5124,22 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="C30" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="G30" s="2">
         <v>0.16666666666666666</v>
@@ -5096,13 +5147,13 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="C31" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>11</v>
@@ -5111,7 +5162,7 @@
         <v>7</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="G31" s="2">
         <v>4.1666666666666664E-2</v>
@@ -5119,22 +5170,22 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="C32" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="G32" s="2">
         <v>4.1666666666666664E-2</v>
@@ -5142,22 +5193,22 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="C33" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="G33" s="2">
         <v>0.125</v>
@@ -5165,22 +5216,22 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="C34" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>28</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="G34" s="2">
         <v>4.1666666666666664E-2</v>
@@ -5188,22 +5239,22 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="C35" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>28</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="G35" s="2">
         <v>6.25E-2</v>
@@ -5211,22 +5262,22 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="C36" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>28</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="G36" s="2">
         <v>2.0833333333333332E-2</v>
@@ -5239,255 +5290,220 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H1:H9"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
-    <col min="5" max="5" width="38.7109375" customWidth="1"/>
-    <col min="6" max="6" width="34.85546875" customWidth="1"/>
-    <col min="7" max="8" width="36.140625" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" customWidth="1"/>
+    <col min="5" max="6" width="36.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:6">
       <c r="B1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" t="s">
         <v>89</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" t="s">
         <v>90</v>
       </c>
-      <c r="D1" t="s">
-        <v>179</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="D2" t="s">
+        <v>174</v>
+      </c>
+      <c r="E2" t="s">
         <v>93</v>
       </c>
-      <c r="F1" t="s">
-        <v>95</v>
-      </c>
-      <c r="G1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D2" t="s">
-        <v>180</v>
-      </c>
-      <c r="E2" t="s">
-        <v>94</v>
-      </c>
       <c r="F2" t="s">
-        <v>94</v>
-      </c>
-      <c r="G2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B3" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C3" s="10">
         <v>41907</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="E3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B4" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C4" s="10">
         <v>41908</v>
       </c>
       <c r="D4" t="s">
-        <v>181</v>
-      </c>
-      <c r="E4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B5" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C5" s="10">
         <v>41909</v>
       </c>
       <c r="D5" t="s">
-        <v>181</v>
-      </c>
-      <c r="E5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B6" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C6" s="10">
         <v>41907</v>
       </c>
       <c r="D6" t="s">
-        <v>181</v>
-      </c>
-      <c r="E6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="B7" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C7" s="10">
         <v>41908</v>
       </c>
       <c r="D7" t="s">
-        <v>181</v>
-      </c>
-      <c r="E7" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="B8" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C8" s="10">
         <v>41910</v>
       </c>
       <c r="D8" t="s">
-        <v>181</v>
-      </c>
-      <c r="E8" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B9" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C9" s="10">
         <v>41883</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>99</v>
+      </c>
+      <c r="E11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
         <v>100</v>
       </c>
-      <c r="G9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="s">
-        <v>102</v>
-      </c>
-      <c r="E10" t="s">
-        <v>103</v>
-      </c>
-      <c r="G10" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" t="s">
-        <v>105</v>
-      </c>
-      <c r="E11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G11" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B13" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C13" s="10">
         <v>41878</v>
       </c>
       <c r="D13" s="10"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B14" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C14" s="10">
         <v>41879</v>
       </c>
       <c r="D14" s="10"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B15" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C15" s="10">
         <v>41880</v>
       </c>
       <c r="D15" s="10"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B16" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C16" s="10">
         <v>41881</v>
@@ -5496,10 +5512,10 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B17" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C17" s="10">
         <v>41882</v>
@@ -5508,10 +5524,10 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B18" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C18" s="10">
         <v>41883</v>
@@ -5520,10 +5536,10 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B19" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C19" s="10">
         <v>41884</v>
@@ -5532,10 +5548,10 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B20" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C20" s="10">
         <v>41885</v>
@@ -5544,10 +5560,10 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B21" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C21" s="10">
         <v>41886</v>
@@ -5556,10 +5572,10 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B22" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C22" s="10">
         <v>41887</v>
@@ -5568,10 +5584,10 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B23" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C23" s="10">
         <v>41888</v>
@@ -5580,10 +5596,10 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B24" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C24" s="10">
         <v>41889</v>
@@ -5592,10 +5608,10 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B25" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C25" s="10">
         <v>41890</v>
@@ -5604,10 +5620,10 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B26" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C26" s="10">
         <v>41891</v>
@@ -5616,10 +5632,10 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B27" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C27" s="10">
         <v>41892</v>
@@ -5628,10 +5644,10 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B28" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C28" s="10">
         <v>41893</v>
@@ -5640,10 +5656,10 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B29" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C29" s="10">
         <v>41894</v>
@@ -5652,10 +5668,10 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B30" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C30" s="10">
         <v>41895</v>
@@ -5664,10 +5680,10 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B31" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C31" s="10">
         <v>41896</v>
@@ -5676,10 +5692,10 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B32" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C32" s="10">
         <v>41897</v>
@@ -5688,10 +5704,10 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B33" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C33" s="10">
         <v>41898</v>
@@ -5700,10 +5716,10 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B34" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C34" s="10">
         <v>41899</v>
@@ -5712,10 +5728,10 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B35" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C35" s="10">
         <v>41900</v>
@@ -5724,10 +5740,10 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
+        <v>122</v>
+      </c>
+      <c r="B36" t="s">
         <v>128</v>
-      </c>
-      <c r="B36" t="s">
-        <v>134</v>
       </c>
       <c r="C36" s="10">
         <v>41901</v>
@@ -5736,10 +5752,10 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B37" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C37" s="10">
         <v>41902</v>
@@ -5748,10 +5764,10 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B38" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C38" s="10">
         <v>41903</v>
@@ -5760,10 +5776,10 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B39" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C39" s="10">
         <v>41904</v>
@@ -5772,10 +5788,10 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B40" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C40" s="10">
         <v>41905</v>
@@ -5784,10 +5800,10 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B41" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C41" s="10">
         <v>41906</v>
@@ -5804,15 +5820,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -5820,35 +5836,40 @@
         <v>65</v>
       </c>
       <c r="B1" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="C1" t="s">
-        <v>183</v>
+        <v>177</v>
+      </c>
+      <c r="D1" t="s">
+        <v>241</v>
+      </c>
+      <c r="E1" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>184</v>
-      </c>
       <c r="C2" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="D2" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>50</v>
-      </c>
+        <v>176</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
       <c r="D3" s="2" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -5858,16 +5879,16 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="4" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="B4" s="4">
         <v>8401</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -5877,7 +5898,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="4" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="B5" s="4">
         <v>8411</v>
@@ -5886,7 +5907,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -5896,16 +5917,12 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>50</v>
-      </c>
+        <v>231</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
       <c r="D6" s="2" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -5913,7 +5930,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="4" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="B7" s="4">
         <v>8361</v>
@@ -5922,7 +5939,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -5930,7 +5947,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="4" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="B8" s="4">
         <v>8341</v>
@@ -5939,7 +5956,7 @@
         <v>2</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -5947,26 +5964,26 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="4" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="B9" s="4">
         <v>8401</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="4" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="B10" s="4">
         <v>8341</v>
@@ -5975,7 +5992,7 @@
         <v>2</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -5983,7 +6000,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="4" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="B11" s="4">
         <v>8331</v>
@@ -5992,7 +6009,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -6000,7 +6017,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="4" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="B12" s="4">
         <v>8341</v>
@@ -6009,7 +6026,7 @@
         <v>2.5</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -6017,16 +6034,16 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="4" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="B13" s="4">
         <v>8361</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
     </row>
     <row r="14" spans="1:9">

</xml_diff>